<commit_message>
Prepare for deployment to Streamlit Cloud
</commit_message>
<xml_diff>
--- a/data_calculated.xlsx
+++ b/data_calculated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Documents/pythonProject/calculator_pileg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100D12CE-D148-B64F-95C3-ADF231B5EE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B46872D-9E3E-7D4B-9850-973395693E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="3" xr2:uid="{21A968B2-5339-AD4E-85AA-F71C63B86228}"/>
   </bookViews>
@@ -17,7 +17,11 @@
     <sheet name="dapil" sheetId="2" r:id="rId2"/>
     <sheet name="hasil_sl" sheetId="3" r:id="rId3"/>
     <sheet name="detail_sl" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">dapil!$A$1:$F$85</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2199" uniqueCount="713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2319" uniqueCount="751">
   <si>
     <t>DAPIL</t>
   </si>
@@ -2183,6 +2187,120 @@
   </si>
   <si>
     <t>URUTAN KURSI</t>
+  </si>
+  <si>
+    <t>Jatim:</t>
+  </si>
+  <si>
+    <t>1.⁠ ⁠Dapil 1 (tandem PKB)</t>
+  </si>
+  <si>
+    <t>2.⁠ ⁠⁠Dapil 2 (Faisol Riza, Mufti Anam)</t>
+  </si>
+  <si>
+    <t>3.⁠ ⁠⁠Dapil 3 (Inna Amania/PDIP)</t>
+  </si>
+  <si>
+    <t>4.⁠ ⁠⁠Dapil 4 (Rifqy/tandem PKB)</t>
+  </si>
+  <si>
+    <t>5.⁠ ⁠⁠Dapil 5 (Rino Lande)</t>
+  </si>
+  <si>
+    <t>6.⁠ ⁠⁠Dapil 6 (Mas Abu)</t>
+  </si>
+  <si>
+    <t>7.⁠ ⁠⁠Dapil 7 (Ahmad Iman Sukri/PKB)</t>
+  </si>
+  <si>
+    <t>8.⁠ ⁠⁠Dapil 8 (RK, GH dan tandem PKB)</t>
+  </si>
+  <si>
+    <t>Jateng:</t>
+  </si>
+  <si>
+    <t>1.⁠ ⁠Dapil 1 (Firly Ganinduto/putus kontrak)</t>
+  </si>
+  <si>
+    <t>2.⁠ ⁠⁠Dapil 2 (Hindun PKB)</t>
+  </si>
+  <si>
+    <t>2.⁠ ⁠Dapil 6 (Gus Abdu/PKB)</t>
+  </si>
+  <si>
+    <t>3.⁠ ⁠⁠Dapil 10 (Dito Ganinduto/putus kontrak)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIY: </t>
+  </si>
+  <si>
+    <t>1.⁠ ⁠Arnanto/PG</t>
+  </si>
+  <si>
+    <t>JABAR:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.⁠ ⁠Dapil 1 </t>
+  </si>
+  <si>
+    <t>2.⁠ ⁠⁠Dapil 10 Rina</t>
+  </si>
+  <si>
+    <t>Sumsel:</t>
+  </si>
+  <si>
+    <t>1.⁠ ⁠Dapil 1 (CU)</t>
+  </si>
+  <si>
+    <t>2.⁠ ⁠⁠Dapil 2 (bobby)</t>
+  </si>
+  <si>
+    <t>Kaltim:</t>
+  </si>
+  <si>
+    <t>1.⁠ ⁠Hetifah</t>
+  </si>
+  <si>
+    <t>NTT:</t>
+  </si>
+  <si>
+    <t>1.⁠ ⁠Dapil 1 (Dipo/PKB)</t>
+  </si>
+  <si>
+    <t>NTB:</t>
+  </si>
+  <si>
+    <t>1.⁠ ⁠Dapil 1 (lalu ari)</t>
+  </si>
+  <si>
+    <t>2.⁠ ⁠⁠Dapil 2 (magdalena)</t>
+  </si>
+  <si>
+    <t>Sumut:</t>
+  </si>
+  <si>
+    <t>1.⁠ ⁠Dapil 1 (Meutya)</t>
+  </si>
+  <si>
+    <t>Riau</t>
+  </si>
+  <si>
+    <t>1.⁠ ⁠Dapil 1 (Iyeth Bustami)</t>
+  </si>
+  <si>
+    <t>Kepri</t>
+  </si>
+  <si>
+    <t>1.⁠ ⁠Cen sui lan (PG)</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>TERDAPAT CLIENT PUSDEHAM PADA PEMILU 2024</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -2251,7 +2369,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -2271,6 +2389,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -7651,10 +7775,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD1EE29-32D3-6B4C-AE7E-0EDD8A4FD907}">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7662,9 +7786,10 @@
     <col min="1" max="3" width="24.33203125" customWidth="1"/>
     <col min="4" max="4" width="24.33203125" style="8" customWidth="1"/>
     <col min="5" max="5" width="24.33203125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="43.33203125" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -7680,8 +7805,11 @@
       <c r="E1" s="9" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="4" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -7697,8 +7825,11 @@
       <c r="E2" s="2">
         <v>2289115</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -7714,8 +7845,11 @@
       <c r="E3" s="2">
         <v>3973080</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -7731,8 +7865,11 @@
       <c r="E4" s="2">
         <v>2632764</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -7748,8 +7885,11 @@
       <c r="E5" s="2">
         <v>2255850</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -7765,8 +7905,11 @@
       <c r="E6" s="2">
         <v>3889441</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -7782,8 +7925,11 @@
       <c r="E7" s="2">
         <v>3202856</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -7799,8 +7945,11 @@
       <c r="E8" s="2">
         <v>4713343</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -7816,8 +7965,11 @@
       <c r="E9" s="2">
         <v>3360658</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -7833,8 +7985,11 @@
       <c r="E10" s="2">
         <v>3088907</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -7850,8 +8005,11 @@
       <c r="E11" s="2">
         <v>2348025</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -7867,8 +8025,11 @@
       <c r="E12" s="2">
         <v>3960862</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -7884,8 +8045,11 @@
       <c r="E13" s="2">
         <v>2676107</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -7901,8 +8065,11 @@
       <c r="E14" s="2">
         <v>881206</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -7918,8 +8085,11 @@
       <c r="E15" s="2">
         <v>2870974</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -7935,8 +8105,11 @@
       <c r="E16" s="2">
         <v>2383972</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -7952,8 +8125,11 @@
       <c r="E17" s="2">
         <v>4346875</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -7969,8 +8145,11 @@
       <c r="E18" s="2">
         <v>3272524</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -7986,8 +8165,11 @@
       <c r="E19" s="2">
         <v>3269516</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -8003,8 +8185,11 @@
       <c r="E20" s="2">
         <v>1964576</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -8020,8 +8205,11 @@
       <c r="E21" s="2">
         <v>1777461</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -8037,8 +8225,11 @@
       <c r="E22" s="2">
         <v>1494828</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -8054,8 +8245,11 @@
       <c r="E23" s="2">
         <v>2044770</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -8071,8 +8265,11 @@
       <c r="E24" s="2">
         <v>2059041</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -8088,8 +8285,11 @@
       <c r="E25" s="2">
         <v>4738835</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -8105,8 +8305,11 @@
       <c r="E26" s="2">
         <v>2763848</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -8122,8 +8325,11 @@
       <c r="E27" s="2">
         <v>1968326</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -8139,8 +8345,11 @@
       <c r="E28" s="2">
         <v>985760</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -8156,8 +8365,11 @@
       <c r="E29" s="2">
         <v>2375153</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -8173,8 +8385,11 @@
       <c r="E30" s="2">
         <v>2375339</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -8190,8 +8405,11 @@
       <c r="E31" s="2">
         <v>1920090</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -8207,8 +8425,11 @@
       <c r="E32" s="2">
         <v>2236703</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -8224,8 +8445,11 @@
       <c r="E33" s="2">
         <v>1867931</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -8241,8 +8465,11 @@
       <c r="E34" s="2">
         <v>1969603</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -8258,8 +8485,11 @@
       <c r="E35" s="2">
         <v>2298162</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -8275,8 +8505,11 @@
       <c r="E36" s="2">
         <v>1790444</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -8292,8 +8525,11 @@
       <c r="E37" s="2">
         <v>2952030</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" s="12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -8309,8 +8545,11 @@
       <c r="E38" s="2">
         <v>3374318</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" s="12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -8326,8 +8565,11 @@
       <c r="E39" s="2">
         <v>3895322</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" s="12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -8343,8 +8585,11 @@
       <c r="E40" s="2">
         <v>3438838</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
@@ -8360,8 +8605,11 @@
       <c r="E41" s="2">
         <v>3519780</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -8377,8 +8625,11 @@
       <c r="E42" s="2">
         <v>2985146</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" s="12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -8394,8 +8645,11 @@
       <c r="E43" s="2">
         <v>2454563</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" s="12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
@@ -8411,8 +8665,11 @@
       <c r="E44" s="2">
         <v>3366140</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
@@ -8428,8 +8685,11 @@
       <c r="E45" s="2">
         <v>2313625</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
@@ -8445,8 +8705,11 @@
       <c r="E46" s="2">
         <v>2914733</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
@@ -8462,8 +8725,11 @@
       <c r="E47" s="2">
         <v>3030588</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" s="12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
@@ -8479,8 +8745,11 @@
       <c r="E48" s="2">
         <v>2642386</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
@@ -8496,8 +8765,11 @@
       <c r="E49" s="2">
         <v>2889101</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
@@ -8513,8 +8785,11 @@
       <c r="E50" s="2">
         <v>2966971</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
@@ -8530,8 +8805,11 @@
       <c r="E51" s="2">
         <v>2726160</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
@@ -8547,8 +8825,11 @@
       <c r="E52" s="2">
         <v>3680228</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52" s="12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
@@ -8564,8 +8845,11 @@
       <c r="E53" s="2">
         <v>2422268</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" s="12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
@@ -8581,8 +8865,11 @@
       <c r="E54" s="2">
         <v>2464420</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54" s="12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
@@ -8598,8 +8885,11 @@
       <c r="E55" s="2">
         <v>2809882</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55" s="12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
@@ -8615,8 +8905,11 @@
       <c r="E56" s="2">
         <v>2870452</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" s="12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
@@ -8632,8 +8925,11 @@
       <c r="E57" s="2">
         <v>3431669</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57" s="12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
@@ -8649,8 +8945,11 @@
       <c r="E58" s="2">
         <v>3059436</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58" s="12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
@@ -8666,8 +8965,11 @@
       <c r="E59" s="2">
         <v>3549110</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59" s="12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
@@ -8683,8 +8985,11 @@
       <c r="E60" s="2">
         <v>1979375</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
@@ -8700,8 +9005,11 @@
       <c r="E61" s="2">
         <v>2006768</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
@@ -8717,8 +9025,11 @@
       <c r="E62" s="2">
         <v>3129230</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
@@ -8734,8 +9045,11 @@
       <c r="E63" s="2">
         <v>1341012</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
@@ -8751,8 +9065,11 @@
       <c r="E64" s="2">
         <v>953978</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
@@ -8768,8 +9085,11 @@
       <c r="E65" s="2">
         <v>1143741</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65" s="12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
@@ -8785,8 +9105,11 @@
       <c r="E66" s="2">
         <v>2774550</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66" s="12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
@@ -8802,8 +9125,11 @@
       <c r="E67" s="2">
         <v>1824278</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67" s="12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
@@ -8819,8 +9145,11 @@
       <c r="E68" s="2">
         <v>2184197</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
@@ -8836,8 +9165,11 @@
       <c r="E69" s="2">
         <v>727835</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
@@ -8853,8 +9185,11 @@
       <c r="E70" s="2">
         <v>385465</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
@@ -8870,8 +9205,11 @@
       <c r="E71" s="2">
         <v>440826</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
@@ -8887,8 +9225,11 @@
       <c r="E72" s="2">
         <v>1306414</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
@@ -8904,8 +9245,11 @@
       <c r="E73" s="2">
         <v>367269</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F73" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
@@ -8921,8 +9265,11 @@
       <c r="E74" s="2">
         <v>1128844</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F74" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
@@ -8938,8 +9285,11 @@
       <c r="E75" s="2">
         <v>3172894</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F75" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>75</v>
       </c>
@@ -8955,8 +9305,11 @@
       <c r="E76" s="2">
         <v>3366234</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F76" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
@@ -8972,8 +9325,11 @@
       <c r="E77" s="2">
         <v>2774586</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F77" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
@@ -8989,8 +9345,11 @@
       <c r="E78" s="2">
         <v>1183975</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F78" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
@@ -9006,8 +9365,11 @@
       <c r="E79" s="2">
         <v>1619098</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F79" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>79</v>
       </c>
@@ -9023,8 +9385,11 @@
       <c r="E80" s="2">
         <v>1406122</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F80" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>80</v>
       </c>
@@ -9040,8 +9405,11 @@
       <c r="E81" s="2">
         <v>1935116</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F81" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>81</v>
       </c>
@@ -9057,8 +9425,11 @@
       <c r="E82" s="2">
         <v>2778644</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F82" s="12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>82</v>
       </c>
@@ -9074,8 +9445,11 @@
       <c r="E83" s="2">
         <v>504252</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F83" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>83</v>
       </c>
@@ -9091,8 +9465,11 @@
       <c r="E84" s="2">
         <v>1067434</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F84" s="12" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>84</v>
       </c>
@@ -9107,6 +9484,9 @@
       </c>
       <c r="E85" s="2">
         <v>1500974</v>
+      </c>
+      <c r="F85" s="12" t="s">
+        <v>748</v>
       </c>
     </row>
   </sheetData>
@@ -11602,7 +11982,7 @@
   <dimension ref="A1:F581"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23238,4 +23618,194 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E44DD29-6BAD-DC4D-AC75-7F5DF179CBA5}">
+  <dimension ref="A1:A45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>747</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>